<commit_message>
bug fixed for TranscriptField
</commit_message>
<xml_diff>
--- a/client/fusionai cost.xlsx
+++ b/client/fusionai cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchau/Documents/Projects/Video Summarizer/client/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909DEF30-E039-5342-8FF6-EE619AB07F73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D37A8-1F36-3A43-B559-2AC4E57BFBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24220" yWindow="2360" windowWidth="35540" windowHeight="37220" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
+    <workbookView xWindow="13900" yWindow="3380" windowWidth="34960" windowHeight="28720" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>money</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>Factor</t>
+  </si>
+  <si>
+    <t>GPU runtime</t>
+  </si>
+  <si>
+    <t>video length</t>
+  </si>
+  <si>
+    <t>concurrent</t>
   </si>
 </sst>
 </file>
@@ -218,7 +227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,15 +562,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451ABE5E-79CB-48A6-B8FF-3B3BF6DDBD75}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
@@ -738,7 +749,7 @@
         <f>C6*100</f>
         <v>35.909999999999997</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="1">
         <v>14500</v>
       </c>
       <c r="F6">
@@ -755,6 +766,50 @@
       <c r="I6" s="5">
         <f>H6*100</f>
         <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="19">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="19">
+        <v>5.2083333333333336E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="19">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" s="19">
+        <v>9.930555555555555E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="19">
+        <v>0.7368055555555556</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="19">
+        <v>0.13541666666666666</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allow transcript options, and save transcript results to the database
</commit_message>
<xml_diff>
--- a/client/fusionai cost.xlsx
+++ b/client/fusionai cost.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchau/Documents/Projects/Video Summarizer/client/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Video-Summarizer\client\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67D37A8-1F36-3A43-B559-2AC4E57BFBB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD51026-30FE-49AA-93D3-1819F369D995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13900" yWindow="3380" windowWidth="34960" windowHeight="28720" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
+    <workbookView xWindow="450" yWindow="16125" windowWidth="19230" windowHeight="16200" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$22:$N$33</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>money</t>
   </si>
@@ -75,6 +78,33 @@
   </si>
   <si>
     <t>concurrent</t>
+  </si>
+  <si>
+    <t>factor</t>
+  </si>
+  <si>
+    <t>OPENAI</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>3090 HOME</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>credits/dollar</t>
+  </si>
+  <si>
+    <t>profit margin factor</t>
+  </si>
+  <si>
+    <t>cost/t</t>
   </si>
 </sst>
 </file>
@@ -86,13 +116,18 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -201,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -218,6 +253,7 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -227,7 +263,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -562,32 +604,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451ABE5E-79CB-48A6-B8FF-3B3BF6DDBD75}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B1" s="16" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="16" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
@@ -595,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -625,7 +670,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>12.5</v>
       </c>
@@ -661,7 +706,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8.5</v>
       </c>
@@ -697,7 +742,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>14.9</v>
       </c>
@@ -733,7 +778,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>39.9</v>
       </c>
@@ -768,7 +813,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -779,44 +824,606 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="19">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="16">
         <v>0.7368055555555556</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="16">
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="19">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>0.7368055555555556</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" s="19">
+      <c r="C15" s="16">
         <v>9.930555555555555E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="19">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>0.7368055555555556</v>
       </c>
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="C16" s="19">
+      <c r="C16" s="16">
         <v>0.13541666666666666</v>
       </c>
     </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>19</v>
+      </c>
+      <c r="I20">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="N21">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>14</v>
+      </c>
+      <c r="K22" t="s">
+        <v>18</v>
+      </c>
+      <c r="L22" t="s">
+        <v>13</v>
+      </c>
+      <c r="M22" t="s">
+        <v>2</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>147</v>
+      </c>
+      <c r="B23" s="4">
+        <f>A23/3600</f>
+        <v>4.0833333333333333E-2</v>
+      </c>
+      <c r="C23" s="21" t="str">
+        <f>TEXT(A23/86400, "hh:mm:ss")</f>
+        <v>00:02:27</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>12</v>
+      </c>
+      <c r="F23" s="22" t="str">
+        <f>TEXT(E23/86400, "hh:mm:ss")</f>
+        <v>00:00:12</v>
+      </c>
+      <c r="G23" s="2">
+        <f>E23/A23</f>
+        <v>8.1632653061224483E-2</v>
+      </c>
+      <c r="H23" s="2">
+        <f>E23/60*(0.25/60)/D23</f>
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="I23" s="20">
+        <f>H23*$I$20*$I$21</f>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="M23" s="2">
+        <f>0.006*A23/60</f>
+        <v>1.47E-2</v>
+      </c>
+      <c r="N23" s="20">
+        <f>M23*$I$20*$N$21</f>
+        <v>1.5434999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>512</v>
+      </c>
+      <c r="B24" s="4">
+        <f>A24/3600</f>
+        <v>0.14222222222222222</v>
+      </c>
+      <c r="C24" s="21" t="str">
+        <f>TEXT(A24/86400, "hh:mm:ss")</f>
+        <v>00:08:32</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>58</v>
+      </c>
+      <c r="F24" s="22" t="str">
+        <f>TEXT(E24/86400, "hh:mm:ss")</f>
+        <v>00:00:58</v>
+      </c>
+      <c r="G24" s="2">
+        <f>E24/A24</f>
+        <v>0.11328125</v>
+      </c>
+      <c r="H24" s="2">
+        <f>E24/60*(0.25/60)/D24</f>
+        <v>4.0277777777777777E-3</v>
+      </c>
+      <c r="I24" s="20">
+        <f>H24*$I$20*$I$21</f>
+        <v>1.1277777777777778</v>
+      </c>
+      <c r="M24" s="2">
+        <f>0.006*A24/60</f>
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="N24" s="20">
+        <f>M24*$I$20*$N$21</f>
+        <v>5.3760000000000003</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>512</v>
+      </c>
+      <c r="B25" s="4">
+        <f>A25/3600</f>
+        <v>0.14222222222222222</v>
+      </c>
+      <c r="C25" s="21" t="str">
+        <f>TEXT(A25/86400, "hh:mm:ss")</f>
+        <v>00:08:32</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>103</v>
+      </c>
+      <c r="F25" s="22" t="str">
+        <f>TEXT(E25/86400, "hh:mm:ss")</f>
+        <v>00:01:43</v>
+      </c>
+      <c r="G25" s="2">
+        <f>E25/A25</f>
+        <v>0.201171875</v>
+      </c>
+      <c r="H25" s="2">
+        <f>E25/60*(0.25/60)/D25</f>
+        <v>3.5763888888888885E-3</v>
+      </c>
+      <c r="I25" s="20">
+        <f>H25*$I$20*$I$21</f>
+        <v>1.0013888888888889</v>
+      </c>
+      <c r="M25" s="2">
+        <f>0.006*A25/60</f>
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="N25" s="20">
+        <f>M25*$I$20*$N$21</f>
+        <v>5.3760000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>512</v>
+      </c>
+      <c r="B26" s="4">
+        <f>A26/3600</f>
+        <v>0.14222222222222222</v>
+      </c>
+      <c r="C26" s="21" t="str">
+        <f>TEXT(A26/86400, "hh:mm:ss")</f>
+        <v>00:08:32</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>180</v>
+      </c>
+      <c r="F26" s="22" t="str">
+        <f>TEXT(E26/86400, "hh:mm:ss")</f>
+        <v>00:03:00</v>
+      </c>
+      <c r="G26" s="2">
+        <f>E26/A26</f>
+        <v>0.3515625</v>
+      </c>
+      <c r="H26" s="2">
+        <f>E26/60*(0.25/60)/D26</f>
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I26" s="20">
+        <f>H26*$I$20*$I$21</f>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="M26" s="2">
+        <f>0.006*A26/60</f>
+        <v>5.1200000000000002E-2</v>
+      </c>
+      <c r="N26" s="20">
+        <f>M26*$I$20*$N$21</f>
+        <v>5.3760000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>906</v>
+      </c>
+      <c r="B27" s="4">
+        <f>A27/3600</f>
+        <v>0.25166666666666665</v>
+      </c>
+      <c r="C27" s="21" t="str">
+        <f>TEXT(A27/86400, "hh:mm:ss")</f>
+        <v>00:15:06</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>144</v>
+      </c>
+      <c r="F27" s="22" t="str">
+        <f>TEXT(E27/86400, "hh:mm:ss")</f>
+        <v>00:02:24</v>
+      </c>
+      <c r="G27" s="2">
+        <f>E27/A27</f>
+        <v>0.15894039735099338</v>
+      </c>
+      <c r="H27" s="2">
+        <f>E27/60*(0.25/60)/D27</f>
+        <v>0.01</v>
+      </c>
+      <c r="I27" s="20">
+        <f>H27*$I$20*$I$21</f>
+        <v>2.8000000000000003</v>
+      </c>
+      <c r="M27" s="2">
+        <f>0.006*A27/60</f>
+        <v>9.06E-2</v>
+      </c>
+      <c r="N27" s="20">
+        <f>M27*$I$20*$N$21</f>
+        <v>9.5129999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>906</v>
+      </c>
+      <c r="B28" s="4">
+        <f>A28/3600</f>
+        <v>0.25166666666666665</v>
+      </c>
+      <c r="C28" s="21" t="str">
+        <f>TEXT(A28/86400, "hh:mm:ss")</f>
+        <v>00:15:06</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
+        <v>286</v>
+      </c>
+      <c r="F28" s="22" t="str">
+        <f>TEXT(E28/86400, "hh:mm:ss")</f>
+        <v>00:04:46</v>
+      </c>
+      <c r="G28" s="2">
+        <f>E28/A28</f>
+        <v>0.31567328918322296</v>
+      </c>
+      <c r="H28" s="2">
+        <f>E28/60*(0.25/60)/D28</f>
+        <v>9.9305555555555553E-3</v>
+      </c>
+      <c r="I28" s="20">
+        <f>H28*$I$20*$I$21</f>
+        <v>2.7805555555555554</v>
+      </c>
+      <c r="M28" s="2">
+        <f>0.006*A28/60</f>
+        <v>9.06E-2</v>
+      </c>
+      <c r="N28" s="20">
+        <f>M28*$I$20*$N$21</f>
+        <v>9.5129999999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>906</v>
+      </c>
+      <c r="B29" s="4">
+        <f>A29/3600</f>
+        <v>0.25166666666666665</v>
+      </c>
+      <c r="C29" s="21" t="str">
+        <f>TEXT(A29/86400, "hh:mm:ss")</f>
+        <v>00:15:06</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="F29" s="22" t="str">
+        <f>TEXT(E29/86400, "hh:mm:ss")</f>
+        <v>00:00:00</v>
+      </c>
+      <c r="G29" s="2">
+        <f>E29/A29</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="2">
+        <f>E29/60*(0.25/60)/D29</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="20">
+        <f>H29*$I$20*$I$21</f>
+        <v>0</v>
+      </c>
+      <c r="M29" s="2">
+        <f>0.006*A29/60</f>
+        <v>9.06E-2</v>
+      </c>
+      <c r="N29" s="20">
+        <f>M29*$I$20*$N$21</f>
+        <v>9.5129999999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>1056</v>
+      </c>
+      <c r="B30" s="4">
+        <f>A30/3600</f>
+        <v>0.29333333333333333</v>
+      </c>
+      <c r="C30" s="21" t="str">
+        <f>TEXT(A30/86400, "hh:mm:ss")</f>
+        <v>00:17:36</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>166</v>
+      </c>
+      <c r="F30" s="22" t="str">
+        <f>TEXT(E30/86400, "hh:mm:ss")</f>
+        <v>00:02:46</v>
+      </c>
+      <c r="G30" s="2">
+        <f>E30/A30</f>
+        <v>0.1571969696969697</v>
+      </c>
+      <c r="H30" s="2">
+        <f>E30/60*(0.25/60)/D30</f>
+        <v>1.1527777777777777E-2</v>
+      </c>
+      <c r="I30" s="20">
+        <f>H30*$I$20*$I$21</f>
+        <v>3.2277777777777779</v>
+      </c>
+      <c r="M30" s="2">
+        <f>0.006*A30/60</f>
+        <v>0.1056</v>
+      </c>
+      <c r="N30" s="20">
+        <f>M30*$I$20*$N$21</f>
+        <v>11.088000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1116</v>
+      </c>
+      <c r="B31" s="4">
+        <f>A31/3600</f>
+        <v>0.31</v>
+      </c>
+      <c r="C31" s="21" t="str">
+        <f>TEXT(A31/86400, "hh:mm:ss")</f>
+        <v>00:18:36</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>166</v>
+      </c>
+      <c r="F31" s="22" t="str">
+        <f>TEXT(E31/86400, "hh:mm:ss")</f>
+        <v>00:02:46</v>
+      </c>
+      <c r="G31" s="2">
+        <f>E31/A31</f>
+        <v>0.14874551971326164</v>
+      </c>
+      <c r="H31" s="2">
+        <f>E31/60*(0.25/60)/D31</f>
+        <v>1.1527777777777777E-2</v>
+      </c>
+      <c r="I31" s="20">
+        <f>H31*$I$20*$I$21</f>
+        <v>3.2277777777777779</v>
+      </c>
+      <c r="J31">
+        <v>72</v>
+      </c>
+      <c r="K31" t="str">
+        <f>TEXT(J31/86400, "hh:mm:ss")</f>
+        <v>00:01:12</v>
+      </c>
+      <c r="L31" s="2">
+        <f>J31/A31</f>
+        <v>6.4516129032258063E-2</v>
+      </c>
+      <c r="M31" s="2">
+        <f>0.006*A31/60</f>
+        <v>0.11159999999999999</v>
+      </c>
+      <c r="N31" s="20">
+        <f>M31*$I$20*$N$21</f>
+        <v>11.718</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3600</v>
+      </c>
+      <c r="B32" s="4">
+        <f>A32/3600</f>
+        <v>1</v>
+      </c>
+      <c r="C32" s="21" t="str">
+        <f>TEXT(A32/86400, "hh:mm:ss")</f>
+        <v>01:00:00</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>480</v>
+      </c>
+      <c r="F32" s="22" t="str">
+        <f>TEXT(E32/86400, "hh:mm:ss")</f>
+        <v>00:08:00</v>
+      </c>
+      <c r="G32" s="2">
+        <f>E32/A32</f>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="H32" s="2">
+        <f>E32/60*(0.25/60)/D32</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="I32" s="20">
+        <f>H32*$I$20*$I$21</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="J32">
+        <v>120</v>
+      </c>
+      <c r="K32" t="str">
+        <f>TEXT(J32/86400, "hh:mm:ss")</f>
+        <v>00:02:00</v>
+      </c>
+      <c r="L32" s="2">
+        <f>J32/A32</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="M32" s="2">
+        <f>0.006*A32/60</f>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="N32" s="20">
+        <f>M32*$I$20*$N$21</f>
+        <v>37.800000000000004</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4263</v>
+      </c>
+      <c r="B33" s="4">
+        <f>A33/3600</f>
+        <v>1.1841666666666666</v>
+      </c>
+      <c r="C33" s="21" t="str">
+        <f>TEXT(A33/86400, "hh:mm:ss")</f>
+        <v>01:11:03</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>584</v>
+      </c>
+      <c r="F33" s="22" t="str">
+        <f>TEXT(E33/86400, "hh:mm:ss")</f>
+        <v>00:09:44</v>
+      </c>
+      <c r="G33" s="2">
+        <f>E33/A33</f>
+        <v>0.13699272812573304</v>
+      </c>
+      <c r="H33" s="2">
+        <f>E33/60*(0.25/60)/D33</f>
+        <v>4.0555555555555553E-2</v>
+      </c>
+      <c r="I33" s="20">
+        <f>H33*$I$20*$I$21</f>
+        <v>11.355555555555554</v>
+      </c>
+      <c r="L33" s="2"/>
+      <c r="M33" s="2">
+        <f>0.006*A33/60</f>
+        <v>0.42630000000000001</v>
+      </c>
+      <c r="N33" s="20">
+        <f>M33*$I$20*$N$21</f>
+        <v>44.761499999999998</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A22:N33" xr:uid="{451ABE5E-79CB-48A6-B8FF-3B3BF6DDBD75}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A23:N33">
+      <sortCondition ref="C22:C33"/>
+    </sortState>
+  </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update site name on google
</commit_message>
<xml_diff>
--- a/client/fusionai cost.xlsx
+++ b/client/fusionai cost.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Video-Summarizer\client\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchau/Documents/Projects/Video Summarizer/client/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4C3A20-CF6D-4E68-8438-111F7512FBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8F8486-61BE-694C-BE08-5A4EEA4FA8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="14820" windowWidth="19230" windowHeight="16200" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
+    <workbookView xWindow="9880" yWindow="880" windowWidth="26120" windowHeight="21220" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -270,6 +270,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,21 +608,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451ABE5E-79CB-48A6-B8FF-3B3BF6DDBD75}">
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
@@ -640,7 +642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>4</v>
       </c>
@@ -670,7 +672,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>12.5</v>
       </c>
@@ -706,7 +708,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>8.5</v>
       </c>
@@ -742,7 +744,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>14.9</v>
       </c>
@@ -778,7 +780,7 @@
       </c>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>39.9</v>
       </c>
@@ -813,7 +815,43 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>146</v>
+      </c>
+      <c r="B7" s="23">
+        <f>0.006*A7</f>
+        <v>0.876</v>
+      </c>
+      <c r="C7" s="4">
+        <f>B7*1.5</f>
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="D7" s="24">
+        <f>C7*100</f>
+        <v>131.4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>54000</v>
+      </c>
+      <c r="F7">
+        <f>15*800</f>
+        <v>12000</v>
+      </c>
+      <c r="G7" s="2">
+        <f>(E7*0.00025+F7*0.00125)/1000</f>
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="H7" s="11">
+        <f>$K$1*G7</f>
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="I7" s="5">
+        <f>H7*100</f>
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -824,7 +862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
         <v>0.7368055555555556</v>
       </c>
@@ -835,7 +873,7 @@
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="16">
         <v>0.7368055555555556</v>
       </c>
@@ -846,7 +884,7 @@
         <v>9.930555555555555E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="16">
         <v>0.7368055555555556</v>
       </c>
@@ -857,7 +895,7 @@
         <v>0.13541666666666666</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H20" t="s">
         <v>19</v>
       </c>
@@ -865,7 +903,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="H21" t="s">
         <v>20</v>
       </c>
@@ -876,7 +914,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -920,7 +958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>147</v>
       </c>
@@ -963,7 +1001,7 @@
         <v>1.5434999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>512</v>
       </c>
@@ -1006,7 +1044,7 @@
         <v>5.3760000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>512</v>
       </c>
@@ -1049,7 +1087,7 @@
         <v>5.3760000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>512</v>
       </c>
@@ -1092,7 +1130,7 @@
         <v>5.3760000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>906</v>
       </c>
@@ -1135,7 +1173,7 @@
         <v>9.5129999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>906</v>
       </c>
@@ -1178,7 +1216,7 @@
         <v>9.5129999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>906</v>
       </c>
@@ -1218,7 +1256,7 @@
         <v>9.5129999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1056</v>
       </c>
@@ -1261,7 +1299,7 @@
         <v>11.088000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1116</v>
       </c>
@@ -1315,7 +1353,7 @@
         <v>11.718</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>3600</v>
       </c>
@@ -1369,7 +1407,7 @@
         <v>37.800000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4263</v>
       </c>
@@ -1413,7 +1451,7 @@
         <v>44.761499999999998</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>585</v>
       </c>

</xml_diff>

<commit_message>
fix bug when no video duration is returned
</commit_message>
<xml_diff>
--- a/client/fusionai cost.xlsx
+++ b/client/fusionai cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchau/Documents/Projects/Video Summarizer/client/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8F8486-61BE-694C-BE08-5A4EEA4FA8EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E144835E-7E38-2C44-8A75-D139C881607B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9880" yWindow="880" windowWidth="26120" windowHeight="21220" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
+    <workbookView xWindow="27960" yWindow="9080" windowWidth="38540" windowHeight="31380" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -236,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -270,8 +270,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +607,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -819,7 +817,7 @@
       <c r="A7">
         <v>146</v>
       </c>
-      <c r="B7" s="23">
+      <c r="B7" s="3">
         <f>0.006*A7</f>
         <v>0.876</v>
       </c>
@@ -827,28 +825,29 @@
         <f>B7*1.5</f>
         <v>1.3140000000000001</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="5">
         <f>C7*100</f>
         <v>131.4</v>
       </c>
       <c r="E7" s="1">
-        <v>54000</v>
+        <f>54000+4500</f>
+        <v>58500</v>
       </c>
       <c r="F7">
-        <f>15*800</f>
-        <v>12000</v>
+        <f>15*800+800</f>
+        <v>12800</v>
       </c>
       <c r="G7" s="2">
         <f>(E7*0.00025+F7*0.00125)/1000</f>
-        <v>2.8500000000000001E-2</v>
+        <v>3.0624999999999999E-2</v>
       </c>
       <c r="H7" s="11">
         <f>$K$1*G7</f>
-        <v>5.7000000000000002E-2</v>
+        <v>6.1249999999999999E-2</v>
       </c>
       <c r="I7" s="5">
         <f>H7*100</f>
-        <v>5.7</v>
+        <v>6.125</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
adjust the cost of fusionai transcription service
</commit_message>
<xml_diff>
--- a/client/fusionai cost.xlsx
+++ b/client/fusionai cost.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonchau/Documents/Projects/Video Summarizer/client/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BA82D2-8411-BB41-AB1C-4FACB0CB5523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BC2968-7A2A-5744-9741-F00D493B4B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20960" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
+    <workbookView xWindow="3940" yWindow="1300" windowWidth="26220" windowHeight="19580" xr2:uid="{73273880-3C7D-462D-97DB-E5F02F0FB4AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{451ABE5E-79CB-48A6-B8FF-3B3BF6DDBD75}">
   <dimension ref="A1:X34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -821,6 +821,14 @@
         <v>0.42500000000000004</v>
       </c>
       <c r="J4" s="1"/>
+      <c r="W4">
+        <f>63/60*25</f>
+        <v>26.25</v>
+      </c>
+      <c r="X4">
+        <f>W4/S3</f>
+        <v>1615.3846153846152</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5">

</xml_diff>